<commit_message>
melhorias na estrutura dos slides
</commit_message>
<xml_diff>
--- a/producao-de-jogos-digitais.xlsx
+++ b/producao-de-jogos-digitais.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salmo\Documents\repos\public-slides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\repos\public-slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8B37DD-BBFE-480D-A9CF-072D8AB6C2E8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="analise-swot" sheetId="1" r:id="rId1"/>
     <sheet name="classificacao-de-riscos" sheetId="2" r:id="rId2"/>
     <sheet name="analise-de-risco" sheetId="3" r:id="rId3"/>
+    <sheet name="descricao-fase-de-conceituacao" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,8 +26,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Administrador</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1 semana após a pré-produção começar</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+4 horas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+3-4 semanas após a aprovação do conceito inicial</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Análise SWOT</t>
   </si>
@@ -102,13 +184,157 @@
   </si>
   <si>
     <t>Estratégias de mitigação</t>
+  </si>
+  <si>
+    <t>Conceito</t>
+  </si>
+  <si>
+    <t>Recursos</t>
+  </si>
+  <si>
+    <t>Estimativa de início</t>
+  </si>
+  <si>
+    <t>Estimativa de finalização</t>
+  </si>
+  <si>
+    <t>Tarefas</t>
+  </si>
+  <si>
+    <t>Brainstorm</t>
+  </si>
+  <si>
+    <t>Conceito inicial</t>
+  </si>
+  <si>
+    <t>Análise competitiva</t>
+  </si>
+  <si>
+    <t>Aprovação do conceito inicial</t>
+  </si>
+  <si>
+    <t>Declaração da missão</t>
+  </si>
+  <si>
+    <t>Cenário do Jogo</t>
+  </si>
+  <si>
+    <t>Mecânica do Jogo</t>
+  </si>
+  <si>
+    <t>Sinopse da história</t>
+  </si>
+  <si>
+    <t>Arte conceitual</t>
+  </si>
+  <si>
+    <t>Elementos de áudio</t>
+  </si>
+  <si>
+    <t>Prototipagem</t>
+  </si>
+  <si>
+    <t>Análise de risco</t>
+  </si>
+  <si>
+    <t>Venda a ideia</t>
+  </si>
+  <si>
+    <t>Lançamento do projeto</t>
+  </si>
+  <si>
+    <t>Designer líder</t>
+  </si>
+  <si>
+    <t>Produtor, marketing</t>
+  </si>
+  <si>
+    <t>O produtor conduz as sessões, a equipe participa</t>
+  </si>
+  <si>
+    <t>O produtor conduz as sessões,a equipe participa</t>
+  </si>
+  <si>
+    <t>O produtor conduz a reunião, os líderes participam</t>
+  </si>
+  <si>
+    <t>Designer líder, artista líder</t>
+  </si>
+  <si>
+    <t>Designer líder, redator</t>
+  </si>
+  <si>
+    <t>Artista líder, artista conceitual</t>
+  </si>
+  <si>
+    <t>Designer líder, designer de som</t>
+  </si>
+  <si>
+    <t>Designer líder, produtor</t>
+  </si>
+  <si>
+    <t>Produtor, líderes</t>
+  </si>
+  <si>
+    <t>Produtor</t>
+  </si>
+  <si>
+    <t>Cronograma geral (dias)</t>
+  </si>
+  <si>
+    <t>tolerância</t>
+  </si>
+  <si>
+    <t>Dados estimados para um ciclo de desenvolvimento de seis meses</t>
+  </si>
+  <si>
+    <t>Discuta os conceitos iniciais do jogo, inclusive o gênero e a plataforma</t>
+  </si>
+  <si>
+    <t>Examine as notas do brainstorm. Defina o conceito inicial, o gênero e a plataforma. Incorpore o feedback da equipe</t>
+  </si>
+  <si>
+    <t>Examine a concorrência atual e potencial, execute a análise SWOT com base no conceito inicial</t>
+  </si>
+  <si>
+    <t>Apresente o conceito inicial, com o gênero e a plataforma, para aprovação. Análise competitiva inicial concluída. Incorpore o feedback da gerência</t>
+  </si>
+  <si>
+    <t>Defina a declaração da missão do jogo.</t>
+  </si>
+  <si>
+    <t>Defina o cenário do jogo, inclusive a aparência</t>
+  </si>
+  <si>
+    <t>Crie a visão geral de como os principais elementos do jogo funcionarão: desafios, recompensas, curvas de aprendizado, esquema de controle, elementos de áudio, ambiente multijogador</t>
+  </si>
+  <si>
+    <t>Crie a história de fundo do jogo, as biografias das personagens, a descrição geral de como a história se desenrola no jogo</t>
+  </si>
+  <si>
+    <t>Crie a arte conceitual do cenário, dos personagens e dos objetos do jogo</t>
+  </si>
+  <si>
+    <t>Crie a visão geral de como o voiceover, os efeitos sonoros e a música serão apresentados no jogo</t>
+  </si>
+  <si>
+    <t>Crie protótipos dos principais elementos do jogo</t>
+  </si>
+  <si>
+    <t>Avalie os riscos do projeto, determine a estratégia de eliminação, divulgue para toda a equipe</t>
+  </si>
+  <si>
+    <t>Apresente todos os principais elementos de jogabilidade para a gerência para aprovação, incorpore seu feedback</t>
+  </si>
+  <si>
+    <t>Reúna-se com a equipe para celebrar a aprovação do conceito. Se estiver trabalhando em um título de console, envie o conceito do jogo para o fabricante do console para aprovação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +365,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -225,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -233,15 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -262,6 +492,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,7 +996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -767,30 +1009,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -861,7 +1103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C33F87-58C0-4A83-88C9-7D6EED1036DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -874,36 +1116,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="5">
         <v>3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10">
+      <c r="A3" s="14"/>
+      <c r="B3" s="7">
         <v>4</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -917,11 +1159,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909AA1B0-D840-4EAB-BB19-EF50E6C8DC5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,72 +1173,440 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15">
+        <v>43412</v>
+      </c>
+      <c r="E4" s="15">
+        <f>WORKDAY(IF(C4 &lt; 1, D4, D4 - 1), C4 * (1 + $I$2))</f>
+        <v>43412</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="15">
+        <f>WORKDAY(E4, 1)</f>
+        <v>43413</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" ref="E5:E17" si="0">WORKDAY(IF(C5 &lt; 1, D5, D5 - 1), C5 * (1 + $I$2))</f>
+        <v>43416</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15">
+        <f>WORKDAY(E5, 1)</f>
+        <v>43417</v>
+      </c>
+      <c r="E6" s="15">
+        <f t="shared" si="0"/>
+        <v>43418</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15">
+        <f>WORKDAY(E6, 1)</f>
+        <v>43419</v>
+      </c>
+      <c r="E7" s="15">
+        <f t="shared" si="0"/>
+        <v>43419</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3">
+        <f>(1 / 24) * 4</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D8" s="15">
+        <f t="shared" ref="D8:D17" si="1">WORKDAY(E7, 1)</f>
+        <v>43420</v>
+      </c>
+      <c r="E8" s="15">
+        <f t="shared" si="0"/>
+        <v>43420</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <f t="shared" si="1"/>
+        <v>43423</v>
+      </c>
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
+        <v>43424</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="15">
+        <f t="shared" si="1"/>
+        <v>43425</v>
+      </c>
+      <c r="E10" s="15">
+        <f t="shared" si="0"/>
+        <v>43427</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <f t="shared" si="1"/>
+        <v>43430</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="0"/>
+        <v>43430</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" si="1"/>
+        <v>43431</v>
+      </c>
+      <c r="E12" s="15">
+        <f t="shared" si="0"/>
+        <v>43432</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
+        <f t="shared" si="1"/>
+        <v>43433</v>
+      </c>
+      <c r="E13" s="15">
+        <f t="shared" si="0"/>
+        <v>43433</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3">
+        <v>7</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="1"/>
+        <v>43434</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
+        <v>43445</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" si="1"/>
+        <v>43446</v>
+      </c>
+      <c r="E15" s="15">
+        <f t="shared" si="0"/>
+        <v>43446</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" si="1"/>
+        <v>43447</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="0"/>
+        <v>43447</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="1"/>
+        <v>43448</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="0"/>
+        <v>43448</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
slides para definição dos recursos do jogo, definição da etapas e produtos
</commit_message>
<xml_diff>
--- a/producao-de-jogos-digitais.xlsx
+++ b/producao-de-jogos-digitais.xlsx
@@ -1,38 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\repos\public-slides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salmo\Documents\repos\public-slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5840A5-717E-4F3C-94B8-DBE4B8F17BCD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analise-swot" sheetId="1" r:id="rId1"/>
     <sheet name="classificacao-de-riscos" sheetId="2" r:id="rId2"/>
     <sheet name="analise-de-risco" sheetId="3" r:id="rId3"/>
     <sheet name="descricao-fase-de-conceituacao" sheetId="4" r:id="rId4"/>
+    <sheet name="lista-mestra-de-recursos" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Administrador</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,14 +116,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>Análise SWOT</t>
   </si>
   <si>
-    <t>O principal concorrente de Dominação é o Jogo da Velha</t>
-  </si>
-  <si>
     <t>Fatores internos</t>
   </si>
   <si>
@@ -147,12 +151,6 @@
     <t>enfatizar esse recurso no plano de marketing</t>
   </si>
   <si>
-    <t>o jogo possui regras mais complexas</t>
-  </si>
-  <si>
-    <t>produzir documentação ilustrada</t>
-  </si>
-  <si>
     <t>exposição de jogos de tabuleiro na biblioteca</t>
   </si>
   <si>
@@ -328,12 +326,78 @@
   </si>
   <si>
     <t>Reúna-se com a equipe para celebrar a aprovação do conceito. Se estiver trabalhando em um título de console, envie o conceito do jogo para o fabricante do console para aprovação</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Recurso</t>
+  </si>
+  <si>
+    <t>Jogabilidade</t>
+  </si>
+  <si>
+    <t>Processo</t>
+  </si>
+  <si>
+    <t>Produção</t>
+  </si>
+  <si>
+    <t>interface de usuário fácil de entender</t>
+  </si>
+  <si>
+    <t>possibilidade dos jogadores personalizarem a aparência dos personagens</t>
+  </si>
+  <si>
+    <t>estabelecer um sistema para a circulação de documentos de design e de atualizações de documentos entre a equipe</t>
+  </si>
+  <si>
+    <t>possibilidade de o jogador contabilizar as partidas vencidas</t>
+  </si>
+  <si>
+    <t>melhorias das questões relacionadas a movimentação do cursor no tabuleiro auxiliar</t>
+  </si>
+  <si>
+    <t>Arte</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Engenharia</t>
+  </si>
+  <si>
+    <t>Analista de Qualidade</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>necessário</t>
+  </si>
+  <si>
+    <t>desejado</t>
+  </si>
+  <si>
+    <t>interessante</t>
+  </si>
+  <si>
+    <t>Planilha de pontuação de recursos para o jogo Jogo da WHIP classificada por pontuação média</t>
+  </si>
+  <si>
+    <t>O principal concorrente do Jogo da WHIP é o Jogo da Velha</t>
+  </si>
+  <si>
+    <t>desenvolver um mecanismo que favoreça a melhor estratégia nas disputas por casas.</t>
+  </si>
+  <si>
+    <t>o fator sorte pode ser determinante e prevalecer às habilidades do jogador.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -460,11 +524,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -493,6 +566,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,8 +578,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,11 +1079,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,85 +1092,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1103,7 +1186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1120,8 +1203,8 @@
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>18</v>
+      <c r="A2" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="5">
         <v>3</v>
@@ -1132,7 +1215,7 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="7">
         <v>4</v>
       </c>
@@ -1142,10 +1225,10 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="12"/>
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1159,7 +1242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1174,19 +1257,19 @@
   <sheetData>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1244,11 +1327,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,16 +1341,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="A2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I2">
         <v>0.2</v>
@@ -1275,330 +1358,330 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>43412</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="12">
         <f>WORKDAY(IF(C4 &lt; 1, D4, D4 - 1), C4 * (1 + $I$2))</f>
         <v>43412</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <f>WORKDAY(E4, 1)</f>
         <v>43413</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <f t="shared" ref="E5:E17" si="0">WORKDAY(IF(C5 &lt; 1, D5, D5 - 1), C5 * (1 + $I$2))</f>
         <v>43416</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <f>WORKDAY(E5, 1)</f>
         <v>43417</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <f t="shared" si="0"/>
         <v>43418</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <f>WORKDAY(E6, 1)</f>
         <v>43419</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>43419</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3">
         <f>(1 / 24) * 4</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <f t="shared" ref="D8:D17" si="1">WORKDAY(E7, 1)</f>
         <v>43420</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <f t="shared" si="0"/>
         <v>43420</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <f t="shared" si="1"/>
         <v>43423</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>43424</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>43425</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <f t="shared" si="0"/>
         <v>43427</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <f t="shared" si="1"/>
         <v>43430</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <f t="shared" si="0"/>
         <v>43430</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <f t="shared" si="1"/>
         <v>43431</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <f t="shared" si="0"/>
         <v>43432</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <f t="shared" si="1"/>
         <v>43433</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <f t="shared" si="0"/>
         <v>43433</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3">
         <v>7</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <f t="shared" si="1"/>
         <v>43434</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <f t="shared" si="0"/>
         <v>43445</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <f t="shared" si="1"/>
         <v>43446</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="12">
         <f t="shared" si="0"/>
         <v>43446</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <f t="shared" si="1"/>
         <v>43447</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="12">
         <f t="shared" si="0"/>
         <v>43447</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <f t="shared" si="1"/>
         <v>43448</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="12">
         <f t="shared" si="0"/>
         <v>43448</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1609,4 +1692,304 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B705EF24-F8F1-4CCF-A3CE-D75C0F555DCD}">
+  <dimension ref="A2:H36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9">
+        <f>AVERAGE(C4:G4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3</v>
+      </c>
+      <c r="H5" s="9">
+        <f>AVERAGE(C5:G5)</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="9">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9">
+        <f>AVERAGE(C6:G6)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="9">
+        <f>AVERAGE(C7:G7)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <f>AVERAGE(C8:G8)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="16"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="16"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="16"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="16"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="16"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="16"/>
+    </row>
+  </sheetData>
+  <sortState ref="A4:H8">
+    <sortCondition descending="1" ref="H4:H8"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>